<commit_message>
Autocomplete field was commenting. Then delete all comments. in PageMaster Component.
</commit_message>
<xml_diff>
--- a/Documents/FinalAPI Status.xlsx
+++ b/Documents/FinalAPI Status.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\Manthan\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ABE7CF-2C16-47F5-8241-1D085738A170}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5655" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DeepManthan" sheetId="1" r:id="rId1"/>
@@ -18,12 +12,12 @@
     <sheet name=" Manthan All Component check Li" sheetId="3" r:id="rId3"/>
     <sheet name="manthan CommonCheck List" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="67">
   <si>
     <t>link</t>
   </si>
@@ -219,16 +213,41 @@
   <si>
     <t>Check Point For list Component</t>
   </si>
+  <si>
+    <t>Pages master</t>
+  </si>
+  <si>
+    <t>Pages List</t>
+  </si>
+  <si>
+    <t>If PageType ID =2  ("Page List") is select then Call List Api and  PageList DropDown Values  Display And ShowMenu Checkbox checked And Dissabled</t>
+  </si>
+  <si>
+    <t>first priority</t>
+  </si>
+  <si>
+    <t>If PageType id =1("add page") is select then PageLis Diplay DropDown Value  = " null", and    ShowMenu chechBox  Enablled</t>
+  </si>
+  <si>
+    <t>After PageAccess DropDown ADD Button Work and dropdown value (IsAccess) add in table</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -339,8 +358,30 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,8 +424,26 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -414,108 +473,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8768,7 +8883,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -8776,7 +8891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -8843,13 +8958,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -9174,7 +9291,7 @@
       <c r="C23" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="48" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -9304,20 +9421,523 @@
         <v>23</v>
       </c>
     </row>
+    <row r="55" spans="2:5" ht="15" customHeight="1">
+      <c r="B55" s="47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="15" customHeight="1">
+      <c r="B56" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="55"/>
+      <c r="E56" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15" customHeight="1">
+      <c r="B57" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="55"/>
+      <c r="E57" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15" customHeight="1">
+      <c r="B58" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="55"/>
+      <c r="E58" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15" customHeight="1">
+      <c r="B59" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="55"/>
+      <c r="E59" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15" customHeight="1">
+      <c r="B60" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60" s="55"/>
+      <c r="E60" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="15" customHeight="1">
+      <c r="B61" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="55"/>
+      <c r="E61" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="15" customHeight="1">
+      <c r="B62" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="55"/>
+      <c r="E62" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="15" customHeight="1">
+      <c r="B63" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="15" customHeight="1">
+      <c r="B64" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1">
+      <c r="B65" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="55"/>
+      <c r="E65" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15" customHeight="1">
+      <c r="B66" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="53"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="53"/>
+    </row>
+    <row r="69" spans="1:7" ht="15" customHeight="1">
+      <c r="E69" s="52"/>
+      <c r="F69" s="52"/>
+      <c r="G69" s="52"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1">
+      <c r="D70" s="49"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" customHeight="1">
+      <c r="B71" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" s="49"/>
+      <c r="E71" s="51"/>
+      <c r="F71" s="52"/>
+      <c r="G71" s="52"/>
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1">
+      <c r="A72" s="52"/>
+      <c r="B72" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="52"/>
+    </row>
+    <row r="73" spans="1:7" ht="15" customHeight="1">
+      <c r="A73" s="52"/>
+      <c r="B73" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" customHeight="1">
+      <c r="A74" s="52"/>
+      <c r="B74" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="52"/>
+    </row>
+    <row r="75" spans="1:7" ht="15" customHeight="1">
+      <c r="A75" s="52"/>
+      <c r="B75" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="55"/>
+      <c r="E75" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="52"/>
+      <c r="G75" s="52"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" customHeight="1">
+      <c r="A76" s="52"/>
+      <c r="B76" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="55"/>
+      <c r="E76" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F76" s="52"/>
+      <c r="G76" s="52"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" customHeight="1">
+      <c r="A77" s="52"/>
+      <c r="B77" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="55"/>
+      <c r="E77" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77" s="52"/>
+      <c r="G77" s="52"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1">
+      <c r="A78" s="52"/>
+      <c r="B78" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" s="55"/>
+      <c r="E78" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78" s="52"/>
+      <c r="G78" s="52"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" customHeight="1">
+      <c r="A79" s="52"/>
+      <c r="B79" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" s="55"/>
+      <c r="E79" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="52"/>
+      <c r="G79" s="52"/>
+    </row>
+    <row r="80" spans="1:7" ht="15" customHeight="1">
+      <c r="A80" s="52"/>
+      <c r="B80" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F80" s="52"/>
+      <c r="G80" s="52"/>
+    </row>
+    <row r="81" spans="1:7" ht="15" customHeight="1">
+      <c r="A81" s="52"/>
+      <c r="B81" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C81" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="52"/>
+      <c r="G81" s="52"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" customHeight="1">
+      <c r="A82" s="52"/>
+      <c r="B82" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D82" s="55"/>
+      <c r="E82" s="55"/>
+      <c r="F82" s="52"/>
+      <c r="G82" s="52"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" customHeight="1">
+      <c r="A83" s="52"/>
+      <c r="B83" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D83" s="55"/>
+      <c r="E83" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="52"/>
+      <c r="G83" s="52"/>
+    </row>
+    <row r="84" spans="1:7" ht="15" customHeight="1">
+      <c r="A84" s="52"/>
+      <c r="B84" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" s="55"/>
+      <c r="E84" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" s="52"/>
+      <c r="G84" s="52"/>
+    </row>
+    <row r="85" spans="1:7" ht="15" customHeight="1">
+      <c r="A85" s="52"/>
+      <c r="B85" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="55"/>
+      <c r="E85" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" s="52"/>
+      <c r="G85" s="52"/>
+    </row>
+    <row r="86" spans="1:7" ht="15" customHeight="1">
+      <c r="A86" s="52"/>
+      <c r="B86" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" s="55"/>
+      <c r="E86" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" customHeight="1">
+      <c r="A87" s="52"/>
+      <c r="B87" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C87" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="55"/>
+      <c r="E87" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+    </row>
+    <row r="88" spans="1:7" ht="15" customHeight="1">
+      <c r="A88" s="52"/>
+      <c r="B88" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F88" s="52"/>
+      <c r="G88" s="52"/>
+    </row>
+    <row r="89" spans="1:7" ht="15" customHeight="1">
+      <c r="A89" s="52"/>
+      <c r="B89" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" s="52"/>
+      <c r="G89" s="52"/>
+    </row>
+    <row r="90" spans="1:7" ht="15" customHeight="1">
+      <c r="A90" s="52"/>
+      <c r="B90" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C90" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F90" s="52"/>
+      <c r="G90" s="52"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" customHeight="1">
+      <c r="A91" s="52"/>
+      <c r="B91" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D91" s="55"/>
+      <c r="E91" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" s="52"/>
+      <c r="G91" s="52"/>
+    </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1">
+      <c r="A92" s="52"/>
+      <c r="B92" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C92" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="55"/>
+      <c r="E92" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F92" s="52"/>
+      <c r="G92" s="52"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" customHeight="1">
+      <c r="A93" s="52"/>
+      <c r="B93" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="55"/>
+      <c r="E93" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F93" s="52"/>
+      <c r="G93" s="52"/>
+    </row>
+    <row r="94" spans="1:7" ht="15" customHeight="1">
+      <c r="A94" s="52"/>
+      <c r="B94" s="55"/>
+      <c r="C94" s="55"/>
+      <c r="D94" s="55"/>
+      <c r="E94" s="55"/>
+      <c r="F94" s="52"/>
+      <c r="G94" s="52"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" customHeight="1">
+      <c r="A95" s="52"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="52"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="52"/>
+      <c r="G95" s="52"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" customHeight="1">
+      <c r="E96" s="63"/>
+      <c r="F96" s="52"/>
+    </row>
+    <row r="101" spans="4:4" ht="15" customHeight="1">
+      <c r="D101" s="52"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="C4:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>